<commit_message>
Update README.md and replace image
</commit_message>
<xml_diff>
--- a/testdata/test3.xlsx
+++ b/testdata/test3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -38,6 +38,13 @@
   </si>
   <si>
     <t xml:space="preserve">price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xlsxsql query -H -o md \
+"SELECT a.id,a.name,b.price
+FROM testdata/test3.xlsx::.C1 AS a 
+LEFT JOIN testdata/test3.xlsx::.F4 AS b 
+ON a.id=b.id" </t>
   </si>
 </sst>
 </file>
@@ -47,7 +54,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Noto Sans CJK JP"/>
@@ -75,8 +82,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Noto Sans CJK JP"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,8 +108,14 @@
         <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF5CE"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -158,6 +177,21 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFED4C05"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFED4C05"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFED4C05"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFED4C05"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -186,7 +220,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -229,6 +263,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -260,7 +298,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFF5CE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -287,7 +325,7 @@
       <rgbColor rgb="FFACB20C"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFE8A202"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFED4C05"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -308,13 +346,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C1:G7"/>
+  <dimension ref="C1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="1" t="s">
@@ -378,7 +416,19 @@
         <v>500</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="91" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C10:G10"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>